<commit_message>
functional cu hotkeys dar urat
</commit_message>
<xml_diff>
--- a/src/Qiosk.App/bin/Release/net8.0-windows7.0/Data/attendees.xlsx
+++ b/src/Qiosk.App/bin/Release/net8.0-windows7.0/Data/attendees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qiosk\src\Qiosk.App\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Qiosk\src\Qiosk.App\bin\Release\net8.0-windows7.0\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C734BEB-EA11-4E31-B915-69D1EED95748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A2D111-FB01-4D74-907F-6867F78D0E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,18 +42,6 @@
     <t>COMPANIE</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Corect-Alpha</t>
-  </si>
-  <si>
-    <t>Primar</t>
-  </si>
-  <si>
-    <t>Siret</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -64,6 +52,18 @@
   </si>
   <si>
     <t>Iasi</t>
+  </si>
+  <si>
+    <t>Raluca</t>
+  </si>
+  <si>
+    <t>Sofrone</t>
+  </si>
+  <si>
+    <t>Team Leader Marketing</t>
+  </si>
+  <si>
+    <t>Quartz Matrix</t>
   </si>
 </sst>
 </file>
@@ -384,11 +384,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
@@ -416,16 +418,16 @@
         <v>10788</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -433,16 +435,16 @@
         <v>10722</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>